<commit_message>
update by Haikun 17042025
</commit_message>
<xml_diff>
--- a/【最後】2025 DZ.xlsx
+++ b/【最後】2025 DZ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HAI_NGUYEN\Desktop\TỔNG KẾT\Github-learn\knowledge-2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19309DBA-92FE-4237-ADA6-24AF3176431E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1038CE-2F4C-4F8D-BC97-E0B6353B0DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1479,7 +1479,28 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1497,17 +1518,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="55" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1521,38 +1536,23 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="55" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1575,16 +1575,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>33867</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>27240</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>169334</xdr:rowOff>
+      <xdr:rowOff>3682</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>221973</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>169334</xdr:rowOff>
+      <xdr:rowOff>3682</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1599,8 +1599,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3860800" y="1286934"/>
-          <a:ext cx="194733" cy="177800"/>
+          <a:off x="2916214" y="1096986"/>
+          <a:ext cx="194733" cy="172279"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1641,16 +1641,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>27241</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>6627</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>33866</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>6625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>221974</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>6627</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>228599</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>6625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1665,7 +1665,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="517571" y="1616766"/>
+          <a:off x="2922840" y="1444486"/>
           <a:ext cx="194733" cy="172278"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -3621,8 +3621,8 @@
   </sheetPr>
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AF21" sqref="AF21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AE5" sqref="AE5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -3644,40 +3644,40 @@
       </c>
     </row>
     <row r="2" spans="1:30" ht="15" customHeight="1">
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="65"/>
-      <c r="X2" s="65"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
+      <c r="V2" s="54"/>
+      <c r="W2" s="54"/>
+      <c r="X2" s="54"/>
     </row>
     <row r="4" spans="1:30" ht="14.25" customHeight="1">
       <c r="A4" s="2"/>
-      <c r="B4" s="56">
+      <c r="B4" s="67">
         <v>45748</v>
       </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
       <c r="G4" s="3">
         <v>20</v>
       </c>
@@ -3685,13 +3685,13 @@
         <v>10</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="56">
+      <c r="J4" s="67">
         <v>45778</v>
       </c>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
+      <c r="K4" s="68"/>
+      <c r="L4" s="68"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="68"/>
       <c r="O4" s="3">
         <v>18</v>
       </c>
@@ -3699,13 +3699,13 @@
         <v>13</v>
       </c>
       <c r="Q4" s="2"/>
-      <c r="R4" s="56">
+      <c r="R4" s="67">
         <v>45809</v>
       </c>
-      <c r="S4" s="57"/>
-      <c r="T4" s="57"/>
-      <c r="U4" s="57"/>
-      <c r="V4" s="57"/>
+      <c r="S4" s="68"/>
+      <c r="T4" s="68"/>
+      <c r="U4" s="68"/>
+      <c r="V4" s="68"/>
       <c r="W4" s="3">
         <v>21</v>
       </c>
@@ -4101,35 +4101,35 @@
       <c r="X10" s="11"/>
     </row>
     <row r="11" spans="1:30" ht="14.25" customHeight="1">
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="60"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="65"/>
       <c r="I11" s="16"/>
-      <c r="J11" s="58" t="s">
+      <c r="J11" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="59"/>
-      <c r="L11" s="59"/>
-      <c r="M11" s="59"/>
-      <c r="N11" s="59"/>
-      <c r="O11" s="59"/>
-      <c r="P11" s="60"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="64"/>
+      <c r="M11" s="64"/>
+      <c r="N11" s="64"/>
+      <c r="O11" s="64"/>
+      <c r="P11" s="65"/>
       <c r="Q11" s="16"/>
-      <c r="R11" s="58" t="s">
+      <c r="R11" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="S11" s="59"/>
-      <c r="T11" s="59"/>
-      <c r="U11" s="59"/>
-      <c r="V11" s="59"/>
-      <c r="W11" s="59"/>
-      <c r="X11" s="60"/>
+      <c r="S11" s="64"/>
+      <c r="T11" s="64"/>
+      <c r="U11" s="64"/>
+      <c r="V11" s="64"/>
+      <c r="W11" s="64"/>
+      <c r="X11" s="65"/>
       <c r="Z11" s="38" t="s">
         <v>44</v>
       </c>
@@ -4138,86 +4138,86 @@
       <c r="B12" s="17">
         <v>29</v>
       </c>
-      <c r="C12" s="63" t="s">
+      <c r="C12" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="50"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="57"/>
       <c r="I12" s="18"/>
       <c r="J12" s="17">
         <v>3</v>
       </c>
-      <c r="K12" s="63" t="s">
+      <c r="K12" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="49"/>
-      <c r="M12" s="49"/>
-      <c r="N12" s="49"/>
-      <c r="O12" s="49"/>
-      <c r="P12" s="50"/>
+      <c r="L12" s="56"/>
+      <c r="M12" s="56"/>
+      <c r="N12" s="56"/>
+      <c r="O12" s="56"/>
+      <c r="P12" s="57"/>
       <c r="Q12" s="18"/>
-      <c r="R12" s="61" t="s">
+      <c r="R12" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="S12" s="49"/>
-      <c r="T12" s="49"/>
-      <c r="U12" s="49"/>
-      <c r="V12" s="49"/>
-      <c r="W12" s="49"/>
-      <c r="X12" s="50"/>
+      <c r="S12" s="56"/>
+      <c r="T12" s="56"/>
+      <c r="U12" s="56"/>
+      <c r="V12" s="56"/>
+      <c r="W12" s="56"/>
+      <c r="X12" s="57"/>
     </row>
     <row r="13" spans="1:30" ht="15" customHeight="1">
       <c r="B13" s="19"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="50"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="57"/>
       <c r="I13" s="18"/>
       <c r="J13" s="20">
         <v>4</v>
       </c>
-      <c r="K13" s="51" t="s">
+      <c r="K13" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="L13" s="52"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="52"/>
-      <c r="O13" s="52"/>
-      <c r="P13" s="53"/>
+      <c r="L13" s="59"/>
+      <c r="M13" s="59"/>
+      <c r="N13" s="59"/>
+      <c r="O13" s="59"/>
+      <c r="P13" s="60"/>
       <c r="Q13" s="18"/>
-      <c r="R13" s="62"/>
-      <c r="S13" s="49"/>
-      <c r="T13" s="49"/>
-      <c r="U13" s="49"/>
-      <c r="V13" s="49"/>
-      <c r="W13" s="49"/>
-      <c r="X13" s="50"/>
+      <c r="R13" s="61"/>
+      <c r="S13" s="56"/>
+      <c r="T13" s="56"/>
+      <c r="U13" s="56"/>
+      <c r="V13" s="56"/>
+      <c r="W13" s="56"/>
+      <c r="X13" s="57"/>
     </row>
     <row r="14" spans="1:30" ht="15" customHeight="1">
       <c r="B14" s="21"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="50"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="57"/>
       <c r="I14" s="18"/>
       <c r="J14" s="22">
         <v>5</v>
       </c>
-      <c r="K14" s="51" t="s">
+      <c r="K14" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="L14" s="52"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="52"/>
-      <c r="O14" s="52"/>
-      <c r="P14" s="53"/>
+      <c r="L14" s="59"/>
+      <c r="M14" s="59"/>
+      <c r="N14" s="59"/>
+      <c r="O14" s="59"/>
+      <c r="P14" s="60"/>
       <c r="Q14" s="18"/>
       <c r="R14" s="23"/>
       <c r="S14" s="24"/>
@@ -4228,33 +4228,33 @@
       <c r="X14" s="25"/>
     </row>
     <row r="15" spans="1:30" ht="13.5" customHeight="1">
-      <c r="B15" s="54"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="53"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="60"/>
       <c r="I15" s="26"/>
       <c r="J15" s="22">
         <v>6</v>
       </c>
-      <c r="K15" s="51" t="s">
+      <c r="K15" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="L15" s="52"/>
-      <c r="M15" s="52"/>
-      <c r="N15" s="52"/>
-      <c r="O15" s="52"/>
-      <c r="P15" s="53"/>
+      <c r="L15" s="59"/>
+      <c r="M15" s="59"/>
+      <c r="N15" s="59"/>
+      <c r="O15" s="59"/>
+      <c r="P15" s="60"/>
       <c r="Q15" s="18"/>
-      <c r="R15" s="54"/>
-      <c r="S15" s="52"/>
-      <c r="T15" s="52"/>
-      <c r="U15" s="52"/>
-      <c r="V15" s="52"/>
-      <c r="W15" s="52"/>
-      <c r="X15" s="53"/>
+      <c r="R15" s="62"/>
+      <c r="S15" s="59"/>
+      <c r="T15" s="59"/>
+      <c r="U15" s="59"/>
+      <c r="V15" s="59"/>
+      <c r="W15" s="59"/>
+      <c r="X15" s="60"/>
       <c r="AA15" s="38" t="s">
         <v>45</v>
       </c>
@@ -4286,13 +4286,13 @@
     </row>
     <row r="17" spans="1:28" ht="14.25" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="56">
+      <c r="B17" s="67">
         <v>45839</v>
       </c>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
+      <c r="C17" s="68"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="68"/>
       <c r="G17" s="3">
         <v>23</v>
       </c>
@@ -4300,13 +4300,13 @@
         <v>8</v>
       </c>
       <c r="I17" s="2"/>
-      <c r="J17" s="56">
+      <c r="J17" s="67">
         <v>45870</v>
       </c>
-      <c r="K17" s="57"/>
-      <c r="L17" s="57"/>
-      <c r="M17" s="57"/>
-      <c r="N17" s="57"/>
+      <c r="K17" s="68"/>
+      <c r="L17" s="68"/>
+      <c r="M17" s="68"/>
+      <c r="N17" s="68"/>
       <c r="O17" s="3">
         <v>16</v>
       </c>
@@ -4314,13 +4314,13 @@
         <v>15</v>
       </c>
       <c r="Q17" s="2"/>
-      <c r="R17" s="56">
+      <c r="R17" s="67">
         <v>45901</v>
       </c>
-      <c r="S17" s="57"/>
-      <c r="T17" s="57"/>
-      <c r="U17" s="57"/>
-      <c r="V17" s="57"/>
+      <c r="S17" s="68"/>
+      <c r="T17" s="68"/>
+      <c r="U17" s="68"/>
+      <c r="V17" s="68"/>
       <c r="W17" s="3">
         <v>22</v>
       </c>
@@ -4522,7 +4522,7 @@
       <c r="X20" s="11">
         <v>13</v>
       </c>
-      <c r="AA20" s="72" t="s">
+      <c r="AA20" s="48" t="s">
         <v>48</v>
       </c>
     </row>
@@ -4743,126 +4743,126 @@
       <c r="X24" s="11"/>
     </row>
     <row r="25" spans="1:28" ht="14.25" customHeight="1">
-      <c r="B25" s="58" t="s">
+      <c r="B25" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="60"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="64"/>
+      <c r="H25" s="65"/>
       <c r="I25" s="16"/>
-      <c r="J25" s="58" t="s">
+      <c r="J25" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="K25" s="59"/>
-      <c r="L25" s="59"/>
-      <c r="M25" s="59"/>
-      <c r="N25" s="59"/>
-      <c r="O25" s="59"/>
-      <c r="P25" s="60"/>
+      <c r="K25" s="64"/>
+      <c r="L25" s="64"/>
+      <c r="M25" s="64"/>
+      <c r="N25" s="64"/>
+      <c r="O25" s="64"/>
+      <c r="P25" s="65"/>
       <c r="Q25" s="16"/>
-      <c r="R25" s="58" t="s">
+      <c r="R25" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="S25" s="59"/>
-      <c r="T25" s="59"/>
-      <c r="U25" s="59"/>
-      <c r="V25" s="59"/>
-      <c r="W25" s="59"/>
-      <c r="X25" s="60"/>
+      <c r="S25" s="64"/>
+      <c r="T25" s="64"/>
+      <c r="U25" s="64"/>
+      <c r="V25" s="64"/>
+      <c r="W25" s="64"/>
+      <c r="X25" s="65"/>
     </row>
     <row r="26" spans="1:28" ht="14.25" customHeight="1">
       <c r="B26" s="17">
         <v>21</v>
       </c>
-      <c r="C26" s="63" t="s">
+      <c r="C26" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="50"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="56"/>
+      <c r="H26" s="57"/>
       <c r="I26" s="18"/>
       <c r="J26" s="17">
         <v>11</v>
       </c>
-      <c r="K26" s="63" t="s">
+      <c r="K26" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="L26" s="49"/>
-      <c r="M26" s="49"/>
-      <c r="N26" s="49"/>
-      <c r="O26" s="49"/>
-      <c r="P26" s="50"/>
+      <c r="L26" s="56"/>
+      <c r="M26" s="56"/>
+      <c r="N26" s="56"/>
+      <c r="O26" s="56"/>
+      <c r="P26" s="57"/>
       <c r="Q26" s="18"/>
       <c r="R26" s="17">
         <v>15</v>
       </c>
-      <c r="S26" s="63" t="s">
+      <c r="S26" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="T26" s="49"/>
-      <c r="U26" s="49"/>
-      <c r="V26" s="49"/>
-      <c r="W26" s="49"/>
-      <c r="X26" s="50"/>
+      <c r="T26" s="56"/>
+      <c r="U26" s="56"/>
+      <c r="V26" s="56"/>
+      <c r="W26" s="56"/>
+      <c r="X26" s="57"/>
     </row>
     <row r="27" spans="1:28" ht="14.25" customHeight="1">
       <c r="B27" s="21"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="50"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="57"/>
       <c r="I27" s="18"/>
-      <c r="J27" s="54"/>
-      <c r="K27" s="52"/>
-      <c r="L27" s="52"/>
-      <c r="M27" s="52"/>
-      <c r="N27" s="52"/>
-      <c r="O27" s="52"/>
-      <c r="P27" s="53"/>
+      <c r="J27" s="62"/>
+      <c r="K27" s="59"/>
+      <c r="L27" s="59"/>
+      <c r="M27" s="59"/>
+      <c r="N27" s="59"/>
+      <c r="O27" s="59"/>
+      <c r="P27" s="60"/>
       <c r="Q27" s="18"/>
       <c r="R27" s="20">
         <v>23</v>
       </c>
-      <c r="S27" s="51" t="s">
+      <c r="S27" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="T27" s="52"/>
-      <c r="U27" s="52"/>
-      <c r="V27" s="52"/>
-      <c r="W27" s="52"/>
-      <c r="X27" s="53"/>
+      <c r="T27" s="59"/>
+      <c r="U27" s="59"/>
+      <c r="V27" s="59"/>
+      <c r="W27" s="59"/>
+      <c r="X27" s="60"/>
     </row>
     <row r="28" spans="1:28" ht="13.5" customHeight="1">
       <c r="B28" s="30"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="52"/>
-      <c r="H28" s="53"/>
+      <c r="C28" s="70"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="60"/>
       <c r="I28" s="26"/>
       <c r="J28" s="30"/>
-      <c r="K28" s="55"/>
-      <c r="L28" s="52"/>
-      <c r="M28" s="52"/>
-      <c r="N28" s="52"/>
-      <c r="O28" s="52"/>
-      <c r="P28" s="53"/>
+      <c r="K28" s="70"/>
+      <c r="L28" s="59"/>
+      <c r="M28" s="59"/>
+      <c r="N28" s="59"/>
+      <c r="O28" s="59"/>
+      <c r="P28" s="60"/>
       <c r="Q28" s="26"/>
-      <c r="R28" s="54"/>
-      <c r="S28" s="52"/>
-      <c r="T28" s="52"/>
-      <c r="U28" s="52"/>
-      <c r="V28" s="52"/>
-      <c r="W28" s="52"/>
-      <c r="X28" s="53"/>
+      <c r="R28" s="62"/>
+      <c r="S28" s="59"/>
+      <c r="T28" s="59"/>
+      <c r="U28" s="59"/>
+      <c r="V28" s="59"/>
+      <c r="W28" s="59"/>
+      <c r="X28" s="60"/>
     </row>
     <row r="29" spans="1:28" ht="6" customHeight="1">
       <c r="B29" s="26"/>
@@ -4891,13 +4891,13 @@
     </row>
     <row r="30" spans="1:28" ht="14.25" customHeight="1">
       <c r="A30" s="2"/>
-      <c r="B30" s="56">
+      <c r="B30" s="67">
         <v>45931</v>
       </c>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="68"/>
+      <c r="E30" s="68"/>
+      <c r="F30" s="68"/>
       <c r="G30" s="3">
         <v>23</v>
       </c>
@@ -4905,13 +4905,13 @@
         <v>8</v>
       </c>
       <c r="I30" s="2"/>
-      <c r="J30" s="56">
+      <c r="J30" s="67">
         <v>45962</v>
       </c>
-      <c r="K30" s="57"/>
-      <c r="L30" s="57"/>
-      <c r="M30" s="57"/>
-      <c r="N30" s="57"/>
+      <c r="K30" s="68"/>
+      <c r="L30" s="68"/>
+      <c r="M30" s="68"/>
+      <c r="N30" s="68"/>
       <c r="O30" s="3">
         <v>20</v>
       </c>
@@ -4919,13 +4919,13 @@
         <v>10</v>
       </c>
       <c r="Q30" s="2"/>
-      <c r="R30" s="56">
+      <c r="R30" s="67">
         <v>45992</v>
       </c>
-      <c r="S30" s="57"/>
-      <c r="T30" s="57"/>
-      <c r="U30" s="57"/>
-      <c r="V30" s="57"/>
+      <c r="S30" s="68"/>
+      <c r="T30" s="68"/>
+      <c r="U30" s="68"/>
+      <c r="V30" s="68"/>
       <c r="W30" s="3">
         <v>20</v>
       </c>
@@ -5339,91 +5339,91 @@
       <c r="X37" s="11"/>
     </row>
     <row r="38" spans="1:28" ht="14.25" customHeight="1">
-      <c r="B38" s="58" t="s">
+      <c r="B38" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="59"/>
-      <c r="D38" s="59"/>
-      <c r="E38" s="59"/>
-      <c r="F38" s="59"/>
-      <c r="G38" s="59"/>
-      <c r="H38" s="60"/>
+      <c r="C38" s="64"/>
+      <c r="D38" s="64"/>
+      <c r="E38" s="64"/>
+      <c r="F38" s="64"/>
+      <c r="G38" s="64"/>
+      <c r="H38" s="65"/>
       <c r="I38" s="16"/>
-      <c r="J38" s="58" t="s">
+      <c r="J38" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="K38" s="59"/>
-      <c r="L38" s="59"/>
-      <c r="M38" s="59"/>
-      <c r="N38" s="59"/>
-      <c r="O38" s="59"/>
-      <c r="P38" s="60"/>
+      <c r="K38" s="64"/>
+      <c r="L38" s="64"/>
+      <c r="M38" s="64"/>
+      <c r="N38" s="64"/>
+      <c r="O38" s="64"/>
+      <c r="P38" s="65"/>
       <c r="Q38" s="16"/>
-      <c r="R38" s="58" t="s">
+      <c r="R38" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="S38" s="59"/>
-      <c r="T38" s="59"/>
-      <c r="U38" s="59"/>
-      <c r="V38" s="59"/>
-      <c r="W38" s="59"/>
-      <c r="X38" s="60"/>
+      <c r="S38" s="64"/>
+      <c r="T38" s="64"/>
+      <c r="U38" s="64"/>
+      <c r="V38" s="64"/>
+      <c r="W38" s="64"/>
+      <c r="X38" s="65"/>
     </row>
     <row r="39" spans="1:28" ht="14.25" customHeight="1">
       <c r="B39" s="17">
         <v>13</v>
       </c>
-      <c r="C39" s="63" t="s">
+      <c r="C39" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="D39" s="49"/>
-      <c r="E39" s="49"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="49"/>
-      <c r="H39" s="50"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="56"/>
+      <c r="G39" s="56"/>
+      <c r="H39" s="57"/>
       <c r="I39" s="18"/>
       <c r="J39" s="17">
         <v>3</v>
       </c>
-      <c r="K39" s="63" t="s">
+      <c r="K39" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="L39" s="49"/>
-      <c r="M39" s="49"/>
-      <c r="N39" s="49"/>
-      <c r="O39" s="49"/>
-      <c r="P39" s="50"/>
+      <c r="L39" s="56"/>
+      <c r="M39" s="56"/>
+      <c r="N39" s="56"/>
+      <c r="O39" s="56"/>
+      <c r="P39" s="57"/>
       <c r="Q39" s="18"/>
-      <c r="R39" s="61" t="s">
+      <c r="R39" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="S39" s="49"/>
-      <c r="T39" s="49"/>
-      <c r="U39" s="49"/>
-      <c r="V39" s="49"/>
-      <c r="W39" s="49"/>
-      <c r="X39" s="50"/>
+      <c r="S39" s="56"/>
+      <c r="T39" s="56"/>
+      <c r="U39" s="56"/>
+      <c r="V39" s="56"/>
+      <c r="W39" s="56"/>
+      <c r="X39" s="57"/>
     </row>
     <row r="40" spans="1:28" ht="14.25" customHeight="1">
       <c r="B40" s="21"/>
-      <c r="C40" s="48"/>
-      <c r="D40" s="49"/>
-      <c r="E40" s="49"/>
-      <c r="F40" s="49"/>
-      <c r="G40" s="49"/>
-      <c r="H40" s="50"/>
+      <c r="C40" s="69"/>
+      <c r="D40" s="56"/>
+      <c r="E40" s="56"/>
+      <c r="F40" s="56"/>
+      <c r="G40" s="56"/>
+      <c r="H40" s="57"/>
       <c r="I40" s="18"/>
       <c r="J40" s="22">
         <v>24</v>
       </c>
-      <c r="K40" s="51" t="s">
+      <c r="K40" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="L40" s="52"/>
-      <c r="M40" s="52"/>
-      <c r="N40" s="52"/>
-      <c r="O40" s="52"/>
-      <c r="P40" s="53"/>
+      <c r="L40" s="59"/>
+      <c r="M40" s="59"/>
+      <c r="N40" s="59"/>
+      <c r="O40" s="59"/>
+      <c r="P40" s="60"/>
       <c r="Q40" s="18"/>
       <c r="R40" s="35"/>
       <c r="S40" s="36"/>
@@ -5434,29 +5434,29 @@
       <c r="X40" s="37"/>
     </row>
     <row r="41" spans="1:28" ht="13.5" customHeight="1">
-      <c r="B41" s="54"/>
-      <c r="C41" s="52"/>
-      <c r="D41" s="52"/>
-      <c r="E41" s="52"/>
-      <c r="F41" s="52"/>
-      <c r="G41" s="52"/>
-      <c r="H41" s="53"/>
+      <c r="B41" s="62"/>
+      <c r="C41" s="59"/>
+      <c r="D41" s="59"/>
+      <c r="E41" s="59"/>
+      <c r="F41" s="59"/>
+      <c r="G41" s="59"/>
+      <c r="H41" s="60"/>
       <c r="I41" s="26"/>
-      <c r="J41" s="54"/>
-      <c r="K41" s="52"/>
-      <c r="L41" s="52"/>
-      <c r="M41" s="52"/>
-      <c r="N41" s="52"/>
-      <c r="O41" s="52"/>
-      <c r="P41" s="53"/>
+      <c r="J41" s="62"/>
+      <c r="K41" s="59"/>
+      <c r="L41" s="59"/>
+      <c r="M41" s="59"/>
+      <c r="N41" s="59"/>
+      <c r="O41" s="59"/>
+      <c r="P41" s="60"/>
       <c r="Q41" s="18"/>
       <c r="R41" s="30"/>
-      <c r="S41" s="55"/>
-      <c r="T41" s="52"/>
-      <c r="U41" s="52"/>
-      <c r="V41" s="52"/>
-      <c r="W41" s="52"/>
-      <c r="X41" s="53"/>
+      <c r="S41" s="70"/>
+      <c r="T41" s="59"/>
+      <c r="U41" s="59"/>
+      <c r="V41" s="59"/>
+      <c r="W41" s="59"/>
+      <c r="X41" s="60"/>
     </row>
     <row r="42" spans="1:28" ht="6" customHeight="1">
       <c r="B42" s="26"/>
@@ -5485,13 +5485,13 @@
     </row>
     <row r="43" spans="1:28" ht="14.25" customHeight="1">
       <c r="A43" s="2"/>
-      <c r="B43" s="56">
+      <c r="B43" s="67">
         <v>46023</v>
       </c>
-      <c r="C43" s="57"/>
-      <c r="D43" s="57"/>
-      <c r="E43" s="57"/>
-      <c r="F43" s="57"/>
+      <c r="C43" s="68"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="68"/>
+      <c r="F43" s="68"/>
       <c r="G43" s="3">
         <v>19</v>
       </c>
@@ -5499,13 +5499,13 @@
         <v>12</v>
       </c>
       <c r="I43" s="2"/>
-      <c r="J43" s="56">
+      <c r="J43" s="67">
         <v>46054</v>
       </c>
-      <c r="K43" s="57"/>
-      <c r="L43" s="57"/>
-      <c r="M43" s="57"/>
-      <c r="N43" s="57"/>
+      <c r="K43" s="68"/>
+      <c r="L43" s="68"/>
+      <c r="M43" s="68"/>
+      <c r="N43" s="68"/>
       <c r="O43" s="3">
         <v>20</v>
       </c>
@@ -5513,13 +5513,13 @@
         <v>8</v>
       </c>
       <c r="Q43" s="2"/>
-      <c r="R43" s="56">
+      <c r="R43" s="67">
         <v>46082</v>
       </c>
-      <c r="S43" s="57"/>
-      <c r="T43" s="57"/>
-      <c r="U43" s="57"/>
-      <c r="V43" s="57"/>
+      <c r="S43" s="68"/>
+      <c r="T43" s="68"/>
+      <c r="U43" s="68"/>
+      <c r="V43" s="68"/>
       <c r="W43" s="3">
         <v>22</v>
       </c>
@@ -5904,130 +5904,130 @@
       <c r="X49" s="11"/>
     </row>
     <row r="50" spans="2:28" ht="13.5" customHeight="1">
-      <c r="B50" s="58" t="s">
+      <c r="B50" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="59"/>
-      <c r="D50" s="59"/>
-      <c r="E50" s="59"/>
-      <c r="F50" s="59"/>
-      <c r="G50" s="59"/>
-      <c r="H50" s="60"/>
+      <c r="C50" s="64"/>
+      <c r="D50" s="64"/>
+      <c r="E50" s="64"/>
+      <c r="F50" s="64"/>
+      <c r="G50" s="64"/>
+      <c r="H50" s="65"/>
       <c r="I50" s="16"/>
-      <c r="J50" s="58" t="s">
+      <c r="J50" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="K50" s="59"/>
-      <c r="L50" s="59"/>
-      <c r="M50" s="59"/>
-      <c r="N50" s="59"/>
-      <c r="O50" s="59"/>
-      <c r="P50" s="60"/>
+      <c r="K50" s="64"/>
+      <c r="L50" s="64"/>
+      <c r="M50" s="64"/>
+      <c r="N50" s="64"/>
+      <c r="O50" s="64"/>
+      <c r="P50" s="65"/>
       <c r="Q50" s="16"/>
-      <c r="R50" s="58" t="s">
+      <c r="R50" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="S50" s="59"/>
-      <c r="T50" s="59"/>
-      <c r="U50" s="59"/>
-      <c r="V50" s="59"/>
-      <c r="W50" s="59"/>
-      <c r="X50" s="60"/>
+      <c r="S50" s="64"/>
+      <c r="T50" s="64"/>
+      <c r="U50" s="64"/>
+      <c r="V50" s="64"/>
+      <c r="W50" s="64"/>
+      <c r="X50" s="65"/>
     </row>
     <row r="51" spans="2:28" ht="13.5" customHeight="1">
       <c r="B51" s="17">
         <v>1</v>
       </c>
-      <c r="C51" s="63" t="s">
+      <c r="C51" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="D51" s="49"/>
-      <c r="E51" s="49"/>
-      <c r="F51" s="49"/>
-      <c r="G51" s="49"/>
-      <c r="H51" s="50"/>
+      <c r="D51" s="56"/>
+      <c r="E51" s="56"/>
+      <c r="F51" s="56"/>
+      <c r="G51" s="56"/>
+      <c r="H51" s="57"/>
       <c r="I51" s="18"/>
       <c r="J51" s="17">
         <v>11</v>
       </c>
-      <c r="K51" s="63" t="s">
+      <c r="K51" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="L51" s="49"/>
-      <c r="M51" s="49"/>
-      <c r="N51" s="49"/>
-      <c r="O51" s="49"/>
-      <c r="P51" s="50"/>
+      <c r="L51" s="56"/>
+      <c r="M51" s="56"/>
+      <c r="N51" s="56"/>
+      <c r="O51" s="56"/>
+      <c r="P51" s="57"/>
       <c r="Q51" s="18"/>
       <c r="R51" s="17">
         <v>20</v>
       </c>
-      <c r="S51" s="63" t="s">
+      <c r="S51" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="T51" s="49"/>
-      <c r="U51" s="49"/>
-      <c r="V51" s="49"/>
-      <c r="W51" s="49"/>
-      <c r="X51" s="50"/>
+      <c r="T51" s="56"/>
+      <c r="U51" s="56"/>
+      <c r="V51" s="56"/>
+      <c r="W51" s="56"/>
+      <c r="X51" s="57"/>
     </row>
     <row r="52" spans="2:28" ht="14.25" customHeight="1">
       <c r="B52" s="22">
         <v>12</v>
       </c>
-      <c r="C52" s="51" t="s">
+      <c r="C52" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="D52" s="52"/>
-      <c r="E52" s="52"/>
-      <c r="F52" s="52"/>
-      <c r="G52" s="52"/>
-      <c r="H52" s="53"/>
+      <c r="D52" s="59"/>
+      <c r="E52" s="59"/>
+      <c r="F52" s="59"/>
+      <c r="G52" s="59"/>
+      <c r="H52" s="60"/>
       <c r="I52" s="18"/>
       <c r="J52" s="17">
         <v>23</v>
       </c>
-      <c r="K52" s="63" t="s">
+      <c r="K52" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="L52" s="49"/>
-      <c r="M52" s="49"/>
-      <c r="N52" s="49"/>
-      <c r="O52" s="49"/>
-      <c r="P52" s="50"/>
+      <c r="L52" s="56"/>
+      <c r="M52" s="56"/>
+      <c r="N52" s="56"/>
+      <c r="O52" s="56"/>
+      <c r="P52" s="57"/>
       <c r="Q52" s="18"/>
-      <c r="R52" s="62"/>
-      <c r="S52" s="49"/>
-      <c r="T52" s="49"/>
-      <c r="U52" s="49"/>
-      <c r="V52" s="49"/>
-      <c r="W52" s="49"/>
-      <c r="X52" s="50"/>
+      <c r="R52" s="61"/>
+      <c r="S52" s="56"/>
+      <c r="T52" s="56"/>
+      <c r="U52" s="56"/>
+      <c r="V52" s="56"/>
+      <c r="W52" s="56"/>
+      <c r="X52" s="57"/>
     </row>
     <row r="53" spans="2:28" ht="13.5" customHeight="1">
-      <c r="B53" s="54"/>
-      <c r="C53" s="52"/>
-      <c r="D53" s="52"/>
-      <c r="E53" s="52"/>
-      <c r="F53" s="52"/>
-      <c r="G53" s="52"/>
-      <c r="H53" s="53"/>
+      <c r="B53" s="62"/>
+      <c r="C53" s="59"/>
+      <c r="D53" s="59"/>
+      <c r="E53" s="59"/>
+      <c r="F53" s="59"/>
+      <c r="G53" s="59"/>
+      <c r="H53" s="60"/>
       <c r="I53" s="18"/>
-      <c r="J53" s="54"/>
-      <c r="K53" s="52"/>
-      <c r="L53" s="52"/>
-      <c r="M53" s="52"/>
-      <c r="N53" s="52"/>
-      <c r="O53" s="52"/>
-      <c r="P53" s="53"/>
+      <c r="J53" s="62"/>
+      <c r="K53" s="59"/>
+      <c r="L53" s="59"/>
+      <c r="M53" s="59"/>
+      <c r="N53" s="59"/>
+      <c r="O53" s="59"/>
+      <c r="P53" s="60"/>
       <c r="Q53" s="26"/>
-      <c r="R53" s="54"/>
-      <c r="S53" s="52"/>
-      <c r="T53" s="52"/>
-      <c r="U53" s="52"/>
-      <c r="V53" s="52"/>
-      <c r="W53" s="52"/>
-      <c r="X53" s="53"/>
+      <c r="R53" s="62"/>
+      <c r="S53" s="59"/>
+      <c r="T53" s="59"/>
+      <c r="U53" s="59"/>
+      <c r="V53" s="59"/>
+      <c r="W53" s="59"/>
+      <c r="X53" s="60"/>
     </row>
     <row r="54" spans="2:28" ht="13.5" customHeight="1">
       <c r="Z54" s="38" t="s">
@@ -6125,11 +6125,11 @@
       <c r="S57" s="43"/>
       <c r="T57" s="43"/>
       <c r="U57" s="43"/>
-      <c r="V57" s="67" t="s">
+      <c r="V57" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="W57" s="68"/>
-      <c r="X57" s="69"/>
+      <c r="W57" s="50"/>
+      <c r="X57" s="51"/>
       <c r="Z57" s="38" t="s">
         <v>39</v>
       </c>
@@ -6148,11 +6148,11 @@
       <c r="S58" s="43"/>
       <c r="T58" s="43"/>
       <c r="U58" s="43"/>
-      <c r="V58" s="70">
+      <c r="V58" s="52">
         <v>0</v>
       </c>
-      <c r="W58" s="68"/>
-      <c r="X58" s="69"/>
+      <c r="W58" s="50"/>
+      <c r="X58" s="51"/>
       <c r="Z58" s="38" t="s">
         <v>40</v>
       </c>
@@ -6163,16 +6163,16 @@
     <row r="59" spans="2:28" ht="13.5" customHeight="1">
       <c r="B59" s="46"/>
       <c r="C59" s="41"/>
-      <c r="O59" s="71"/>
-      <c r="P59" s="65"/>
-      <c r="Q59" s="65"/>
-      <c r="R59" s="65"/>
-      <c r="S59" s="65"/>
-      <c r="T59" s="65"/>
-      <c r="U59" s="65"/>
-      <c r="V59" s="65"/>
-      <c r="W59" s="65"/>
-      <c r="X59" s="65"/>
+      <c r="O59" s="53"/>
+      <c r="P59" s="54"/>
+      <c r="Q59" s="54"/>
+      <c r="R59" s="54"/>
+      <c r="S59" s="54"/>
+      <c r="T59" s="54"/>
+      <c r="U59" s="54"/>
+      <c r="V59" s="54"/>
+      <c r="W59" s="54"/>
+      <c r="X59" s="54"/>
     </row>
     <row r="60" spans="2:28" ht="13.5" customHeight="1">
       <c r="B60" s="46"/>
@@ -7297,24 +7297,40 @@
     <row r="1000" ht="13.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="V57:X57"/>
-    <mergeCell ref="V58:X58"/>
-    <mergeCell ref="O59:X59"/>
-    <mergeCell ref="C51:H51"/>
-    <mergeCell ref="C52:H52"/>
-    <mergeCell ref="K52:P52"/>
-    <mergeCell ref="R52:X52"/>
-    <mergeCell ref="B53:H53"/>
-    <mergeCell ref="J53:P53"/>
-    <mergeCell ref="R53:X53"/>
-    <mergeCell ref="K51:P51"/>
-    <mergeCell ref="S51:X51"/>
-    <mergeCell ref="B38:H38"/>
-    <mergeCell ref="J38:P38"/>
-    <mergeCell ref="R38:X38"/>
-    <mergeCell ref="K39:P39"/>
-    <mergeCell ref="R39:X39"/>
-    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="K40:P40"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="J41:P41"/>
+    <mergeCell ref="S41:X41"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="J43:N43"/>
+    <mergeCell ref="R43:V43"/>
+    <mergeCell ref="B50:H50"/>
+    <mergeCell ref="J50:P50"/>
+    <mergeCell ref="R50:X50"/>
+    <mergeCell ref="J17:N17"/>
+    <mergeCell ref="R17:V17"/>
+    <mergeCell ref="R12:X12"/>
+    <mergeCell ref="R13:X13"/>
+    <mergeCell ref="J25:P25"/>
+    <mergeCell ref="R25:X25"/>
+    <mergeCell ref="K12:P12"/>
+    <mergeCell ref="K13:P13"/>
+    <mergeCell ref="K14:P14"/>
+    <mergeCell ref="K15:P15"/>
+    <mergeCell ref="R15:X15"/>
+    <mergeCell ref="C2:X2"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="J4:N4"/>
+    <mergeCell ref="R4:V4"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="R11:X11"/>
+    <mergeCell ref="J11:P11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B17:F17"/>
     <mergeCell ref="J30:N30"/>
     <mergeCell ref="R30:V30"/>
     <mergeCell ref="B25:H25"/>
@@ -7328,40 +7344,24 @@
     <mergeCell ref="B30:F30"/>
     <mergeCell ref="J27:P27"/>
     <mergeCell ref="K28:P28"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="C2:X2"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="J4:N4"/>
-    <mergeCell ref="R4:V4"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="R11:X11"/>
-    <mergeCell ref="J11:P11"/>
-    <mergeCell ref="J17:N17"/>
-    <mergeCell ref="R17:V17"/>
-    <mergeCell ref="R12:X12"/>
-    <mergeCell ref="R13:X13"/>
-    <mergeCell ref="J25:P25"/>
-    <mergeCell ref="R25:X25"/>
-    <mergeCell ref="K12:P12"/>
-    <mergeCell ref="K13:P13"/>
-    <mergeCell ref="K14:P14"/>
-    <mergeCell ref="K15:P15"/>
-    <mergeCell ref="R15:X15"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="J43:N43"/>
-    <mergeCell ref="R43:V43"/>
-    <mergeCell ref="B50:H50"/>
-    <mergeCell ref="J50:P50"/>
-    <mergeCell ref="R50:X50"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="K40:P40"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="J41:P41"/>
-    <mergeCell ref="S41:X41"/>
+    <mergeCell ref="B38:H38"/>
+    <mergeCell ref="J38:P38"/>
+    <mergeCell ref="R38:X38"/>
+    <mergeCell ref="K39:P39"/>
+    <mergeCell ref="R39:X39"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="V57:X57"/>
+    <mergeCell ref="V58:X58"/>
+    <mergeCell ref="O59:X59"/>
+    <mergeCell ref="C51:H51"/>
+    <mergeCell ref="C52:H52"/>
+    <mergeCell ref="K52:P52"/>
+    <mergeCell ref="R52:X52"/>
+    <mergeCell ref="B53:H53"/>
+    <mergeCell ref="J53:P53"/>
+    <mergeCell ref="R53:X53"/>
+    <mergeCell ref="K51:P51"/>
+    <mergeCell ref="S51:X51"/>
   </mergeCells>
   <phoneticPr fontId="10"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
update file excel of Hai
</commit_message>
<xml_diff>
--- a/【最後】2025 DZ.xlsx
+++ b/【最後】2025 DZ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HAI_NGUYEN\Desktop\TỔNG KẾT\Github-learn\knowledge-2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1038CE-2F4C-4F8D-BC97-E0B6353B0DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CF470C-032E-4B13-9A74-611CEA9E4D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1482,25 +1482,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1518,11 +1500,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="55" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1536,23 +1524,35 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="55" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1576,15 +1576,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>27240</xdr:colOff>
+      <xdr:colOff>40492</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>3682</xdr:rowOff>
+      <xdr:rowOff>156082</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>221973</xdr:colOff>
+      <xdr:colOff>235225</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>3682</xdr:rowOff>
+      <xdr:rowOff>156082</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1599,7 +1599,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2916214" y="1096986"/>
+          <a:off x="2929466" y="1249386"/>
           <a:ext cx="194733" cy="172279"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1641,16 +1641,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>33866</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>6625</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>40493</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>6627</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>228599</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>6625</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>235226</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1665,7 +1665,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2922840" y="1444486"/>
+          <a:off x="4320945" y="1099931"/>
           <a:ext cx="194733" cy="172278"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -3159,16 +3159,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>42334</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>55586</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>8466</xdr:rowOff>
+      <xdr:rowOff>1840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>237067</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>250319</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>8466</xdr:rowOff>
+      <xdr:rowOff>1840</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3183,8 +3183,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3869267" y="1659466"/>
-          <a:ext cx="194733" cy="177800"/>
+          <a:off x="2944560" y="1611979"/>
+          <a:ext cx="194733" cy="172278"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -3226,13 +3226,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>42335</xdr:colOff>
+      <xdr:colOff>35709</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>169334</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>237068</xdr:colOff>
+      <xdr:colOff>230442</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>169334</xdr:rowOff>
     </xdr:to>
@@ -3249,8 +3249,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1710268" y="1286934"/>
-          <a:ext cx="194733" cy="177800"/>
+          <a:off x="1533205" y="1262638"/>
+          <a:ext cx="194733" cy="172279"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -3622,7 +3622,7 @@
   <dimension ref="A1:AD1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AE5" sqref="AE5"/>
+      <selection activeCell="AD17" sqref="AD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -3644,40 +3644,40 @@
       </c>
     </row>
     <row r="2" spans="1:30" ht="15" customHeight="1">
-      <c r="C2" s="72" t="s">
+      <c r="C2" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="54"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="66"/>
+      <c r="X2" s="66"/>
     </row>
     <row r="4" spans="1:30" ht="14.25" customHeight="1">
       <c r="A4" s="2"/>
-      <c r="B4" s="67">
+      <c r="B4" s="57">
         <v>45748</v>
       </c>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
       <c r="G4" s="3">
         <v>20</v>
       </c>
@@ -3685,13 +3685,13 @@
         <v>10</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="67">
+      <c r="J4" s="57">
         <v>45778</v>
       </c>
-      <c r="K4" s="68"/>
-      <c r="L4" s="68"/>
-      <c r="M4" s="68"/>
-      <c r="N4" s="68"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
       <c r="O4" s="3">
         <v>18</v>
       </c>
@@ -3699,13 +3699,13 @@
         <v>13</v>
       </c>
       <c r="Q4" s="2"/>
-      <c r="R4" s="67">
+      <c r="R4" s="57">
         <v>45809</v>
       </c>
-      <c r="S4" s="68"/>
-      <c r="T4" s="68"/>
-      <c r="U4" s="68"/>
-      <c r="V4" s="68"/>
+      <c r="S4" s="58"/>
+      <c r="T4" s="58"/>
+      <c r="U4" s="58"/>
+      <c r="V4" s="58"/>
       <c r="W4" s="3">
         <v>21</v>
       </c>
@@ -4101,35 +4101,35 @@
       <c r="X10" s="11"/>
     </row>
     <row r="11" spans="1:30" ht="14.25" customHeight="1">
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="65"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="61"/>
       <c r="I11" s="16"/>
-      <c r="J11" s="63" t="s">
+      <c r="J11" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="64"/>
-      <c r="L11" s="64"/>
-      <c r="M11" s="64"/>
-      <c r="N11" s="64"/>
-      <c r="O11" s="64"/>
-      <c r="P11" s="65"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
+      <c r="M11" s="60"/>
+      <c r="N11" s="60"/>
+      <c r="O11" s="60"/>
+      <c r="P11" s="61"/>
       <c r="Q11" s="16"/>
-      <c r="R11" s="63" t="s">
+      <c r="R11" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="S11" s="64"/>
-      <c r="T11" s="64"/>
-      <c r="U11" s="64"/>
-      <c r="V11" s="64"/>
-      <c r="W11" s="64"/>
-      <c r="X11" s="65"/>
+      <c r="S11" s="60"/>
+      <c r="T11" s="60"/>
+      <c r="U11" s="60"/>
+      <c r="V11" s="60"/>
+      <c r="W11" s="60"/>
+      <c r="X11" s="61"/>
       <c r="Z11" s="38" t="s">
         <v>44</v>
       </c>
@@ -4138,86 +4138,86 @@
       <c r="B12" s="17">
         <v>29</v>
       </c>
-      <c r="C12" s="55" t="s">
+      <c r="C12" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="57"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="51"/>
       <c r="I12" s="18"/>
       <c r="J12" s="17">
         <v>3</v>
       </c>
-      <c r="K12" s="55" t="s">
+      <c r="K12" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="56"/>
-      <c r="M12" s="56"/>
-      <c r="N12" s="56"/>
-      <c r="O12" s="56"/>
-      <c r="P12" s="57"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="51"/>
       <c r="Q12" s="18"/>
-      <c r="R12" s="66" t="s">
+      <c r="R12" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="S12" s="56"/>
-      <c r="T12" s="56"/>
-      <c r="U12" s="56"/>
-      <c r="V12" s="56"/>
-      <c r="W12" s="56"/>
-      <c r="X12" s="57"/>
+      <c r="S12" s="50"/>
+      <c r="T12" s="50"/>
+      <c r="U12" s="50"/>
+      <c r="V12" s="50"/>
+      <c r="W12" s="50"/>
+      <c r="X12" s="51"/>
     </row>
     <row r="13" spans="1:30" ht="15" customHeight="1">
       <c r="B13" s="19"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="56"/>
-      <c r="H13" s="57"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="51"/>
       <c r="I13" s="18"/>
       <c r="J13" s="20">
         <v>4</v>
       </c>
-      <c r="K13" s="58" t="s">
+      <c r="K13" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="59"/>
-      <c r="O13" s="59"/>
-      <c r="P13" s="60"/>
+      <c r="L13" s="53"/>
+      <c r="M13" s="53"/>
+      <c r="N13" s="53"/>
+      <c r="O13" s="53"/>
+      <c r="P13" s="54"/>
       <c r="Q13" s="18"/>
-      <c r="R13" s="61"/>
-      <c r="S13" s="56"/>
-      <c r="T13" s="56"/>
-      <c r="U13" s="56"/>
-      <c r="V13" s="56"/>
-      <c r="W13" s="56"/>
-      <c r="X13" s="57"/>
+      <c r="R13" s="63"/>
+      <c r="S13" s="50"/>
+      <c r="T13" s="50"/>
+      <c r="U13" s="50"/>
+      <c r="V13" s="50"/>
+      <c r="W13" s="50"/>
+      <c r="X13" s="51"/>
     </row>
     <row r="14" spans="1:30" ht="15" customHeight="1">
       <c r="B14" s="21"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="57"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="51"/>
       <c r="I14" s="18"/>
       <c r="J14" s="22">
         <v>5</v>
       </c>
-      <c r="K14" s="58" t="s">
+      <c r="K14" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="L14" s="59"/>
-      <c r="M14" s="59"/>
-      <c r="N14" s="59"/>
-      <c r="O14" s="59"/>
-      <c r="P14" s="60"/>
+      <c r="L14" s="53"/>
+      <c r="M14" s="53"/>
+      <c r="N14" s="53"/>
+      <c r="O14" s="53"/>
+      <c r="P14" s="54"/>
       <c r="Q14" s="18"/>
       <c r="R14" s="23"/>
       <c r="S14" s="24"/>
@@ -4228,33 +4228,33 @@
       <c r="X14" s="25"/>
     </row>
     <row r="15" spans="1:30" ht="13.5" customHeight="1">
-      <c r="B15" s="62"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="60"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="54"/>
       <c r="I15" s="26"/>
       <c r="J15" s="22">
         <v>6</v>
       </c>
-      <c r="K15" s="58" t="s">
+      <c r="K15" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="59"/>
-      <c r="O15" s="59"/>
-      <c r="P15" s="60"/>
+      <c r="L15" s="53"/>
+      <c r="M15" s="53"/>
+      <c r="N15" s="53"/>
+      <c r="O15" s="53"/>
+      <c r="P15" s="54"/>
       <c r="Q15" s="18"/>
-      <c r="R15" s="62"/>
-      <c r="S15" s="59"/>
-      <c r="T15" s="59"/>
-      <c r="U15" s="59"/>
-      <c r="V15" s="59"/>
-      <c r="W15" s="59"/>
-      <c r="X15" s="60"/>
+      <c r="R15" s="55"/>
+      <c r="S15" s="53"/>
+      <c r="T15" s="53"/>
+      <c r="U15" s="53"/>
+      <c r="V15" s="53"/>
+      <c r="W15" s="53"/>
+      <c r="X15" s="54"/>
       <c r="AA15" s="38" t="s">
         <v>45</v>
       </c>
@@ -4286,13 +4286,13 @@
     </row>
     <row r="17" spans="1:28" ht="14.25" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="67">
+      <c r="B17" s="57">
         <v>45839</v>
       </c>
-      <c r="C17" s="68"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="68"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
       <c r="G17" s="3">
         <v>23</v>
       </c>
@@ -4300,13 +4300,13 @@
         <v>8</v>
       </c>
       <c r="I17" s="2"/>
-      <c r="J17" s="67">
+      <c r="J17" s="57">
         <v>45870</v>
       </c>
-      <c r="K17" s="68"/>
-      <c r="L17" s="68"/>
-      <c r="M17" s="68"/>
-      <c r="N17" s="68"/>
+      <c r="K17" s="58"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="58"/>
+      <c r="N17" s="58"/>
       <c r="O17" s="3">
         <v>16</v>
       </c>
@@ -4314,13 +4314,13 @@
         <v>15</v>
       </c>
       <c r="Q17" s="2"/>
-      <c r="R17" s="67">
+      <c r="R17" s="57">
         <v>45901</v>
       </c>
-      <c r="S17" s="68"/>
-      <c r="T17" s="68"/>
-      <c r="U17" s="68"/>
-      <c r="V17" s="68"/>
+      <c r="S17" s="58"/>
+      <c r="T17" s="58"/>
+      <c r="U17" s="58"/>
+      <c r="V17" s="58"/>
       <c r="W17" s="3">
         <v>22</v>
       </c>
@@ -4743,126 +4743,126 @@
       <c r="X24" s="11"/>
     </row>
     <row r="25" spans="1:28" ht="14.25" customHeight="1">
-      <c r="B25" s="63" t="s">
+      <c r="B25" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="64"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="64"/>
-      <c r="G25" s="64"/>
-      <c r="H25" s="65"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="61"/>
       <c r="I25" s="16"/>
-      <c r="J25" s="63" t="s">
+      <c r="J25" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="K25" s="64"/>
-      <c r="L25" s="64"/>
-      <c r="M25" s="64"/>
-      <c r="N25" s="64"/>
-      <c r="O25" s="64"/>
-      <c r="P25" s="65"/>
+      <c r="K25" s="60"/>
+      <c r="L25" s="60"/>
+      <c r="M25" s="60"/>
+      <c r="N25" s="60"/>
+      <c r="O25" s="60"/>
+      <c r="P25" s="61"/>
       <c r="Q25" s="16"/>
-      <c r="R25" s="63" t="s">
+      <c r="R25" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="S25" s="64"/>
-      <c r="T25" s="64"/>
-      <c r="U25" s="64"/>
-      <c r="V25" s="64"/>
-      <c r="W25" s="64"/>
-      <c r="X25" s="65"/>
+      <c r="S25" s="60"/>
+      <c r="T25" s="60"/>
+      <c r="U25" s="60"/>
+      <c r="V25" s="60"/>
+      <c r="W25" s="60"/>
+      <c r="X25" s="61"/>
     </row>
     <row r="26" spans="1:28" ht="14.25" customHeight="1">
       <c r="B26" s="17">
         <v>21</v>
       </c>
-      <c r="C26" s="55" t="s">
+      <c r="C26" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="56"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="56"/>
-      <c r="H26" s="57"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="51"/>
       <c r="I26" s="18"/>
       <c r="J26" s="17">
         <v>11</v>
       </c>
-      <c r="K26" s="55" t="s">
+      <c r="K26" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="L26" s="56"/>
-      <c r="M26" s="56"/>
-      <c r="N26" s="56"/>
-      <c r="O26" s="56"/>
-      <c r="P26" s="57"/>
+      <c r="L26" s="50"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="50"/>
+      <c r="O26" s="50"/>
+      <c r="P26" s="51"/>
       <c r="Q26" s="18"/>
       <c r="R26" s="17">
         <v>15</v>
       </c>
-      <c r="S26" s="55" t="s">
+      <c r="S26" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="T26" s="56"/>
-      <c r="U26" s="56"/>
-      <c r="V26" s="56"/>
-      <c r="W26" s="56"/>
-      <c r="X26" s="57"/>
+      <c r="T26" s="50"/>
+      <c r="U26" s="50"/>
+      <c r="V26" s="50"/>
+      <c r="W26" s="50"/>
+      <c r="X26" s="51"/>
     </row>
     <row r="27" spans="1:28" ht="14.25" customHeight="1">
       <c r="B27" s="21"/>
-      <c r="C27" s="69"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="56"/>
-      <c r="H27" s="57"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="51"/>
       <c r="I27" s="18"/>
-      <c r="J27" s="62"/>
-      <c r="K27" s="59"/>
-      <c r="L27" s="59"/>
-      <c r="M27" s="59"/>
-      <c r="N27" s="59"/>
-      <c r="O27" s="59"/>
-      <c r="P27" s="60"/>
+      <c r="J27" s="55"/>
+      <c r="K27" s="53"/>
+      <c r="L27" s="53"/>
+      <c r="M27" s="53"/>
+      <c r="N27" s="53"/>
+      <c r="O27" s="53"/>
+      <c r="P27" s="54"/>
       <c r="Q27" s="18"/>
       <c r="R27" s="20">
         <v>23</v>
       </c>
-      <c r="S27" s="58" t="s">
+      <c r="S27" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="T27" s="59"/>
-      <c r="U27" s="59"/>
-      <c r="V27" s="59"/>
-      <c r="W27" s="59"/>
-      <c r="X27" s="60"/>
+      <c r="T27" s="53"/>
+      <c r="U27" s="53"/>
+      <c r="V27" s="53"/>
+      <c r="W27" s="53"/>
+      <c r="X27" s="54"/>
     </row>
     <row r="28" spans="1:28" ht="13.5" customHeight="1">
       <c r="B28" s="30"/>
-      <c r="C28" s="70"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="59"/>
-      <c r="H28" s="60"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="54"/>
       <c r="I28" s="26"/>
       <c r="J28" s="30"/>
-      <c r="K28" s="70"/>
-      <c r="L28" s="59"/>
-      <c r="M28" s="59"/>
-      <c r="N28" s="59"/>
-      <c r="O28" s="59"/>
-      <c r="P28" s="60"/>
+      <c r="K28" s="56"/>
+      <c r="L28" s="53"/>
+      <c r="M28" s="53"/>
+      <c r="N28" s="53"/>
+      <c r="O28" s="53"/>
+      <c r="P28" s="54"/>
       <c r="Q28" s="26"/>
-      <c r="R28" s="62"/>
-      <c r="S28" s="59"/>
-      <c r="T28" s="59"/>
-      <c r="U28" s="59"/>
-      <c r="V28" s="59"/>
-      <c r="W28" s="59"/>
-      <c r="X28" s="60"/>
+      <c r="R28" s="55"/>
+      <c r="S28" s="53"/>
+      <c r="T28" s="53"/>
+      <c r="U28" s="53"/>
+      <c r="V28" s="53"/>
+      <c r="W28" s="53"/>
+      <c r="X28" s="54"/>
     </row>
     <row r="29" spans="1:28" ht="6" customHeight="1">
       <c r="B29" s="26"/>
@@ -4891,13 +4891,13 @@
     </row>
     <row r="30" spans="1:28" ht="14.25" customHeight="1">
       <c r="A30" s="2"/>
-      <c r="B30" s="67">
+      <c r="B30" s="57">
         <v>45931</v>
       </c>
-      <c r="C30" s="68"/>
-      <c r="D30" s="68"/>
-      <c r="E30" s="68"/>
-      <c r="F30" s="68"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
       <c r="G30" s="3">
         <v>23</v>
       </c>
@@ -4905,13 +4905,13 @@
         <v>8</v>
       </c>
       <c r="I30" s="2"/>
-      <c r="J30" s="67">
+      <c r="J30" s="57">
         <v>45962</v>
       </c>
-      <c r="K30" s="68"/>
-      <c r="L30" s="68"/>
-      <c r="M30" s="68"/>
-      <c r="N30" s="68"/>
+      <c r="K30" s="58"/>
+      <c r="L30" s="58"/>
+      <c r="M30" s="58"/>
+      <c r="N30" s="58"/>
       <c r="O30" s="3">
         <v>20</v>
       </c>
@@ -4919,13 +4919,13 @@
         <v>10</v>
       </c>
       <c r="Q30" s="2"/>
-      <c r="R30" s="67">
+      <c r="R30" s="57">
         <v>45992</v>
       </c>
-      <c r="S30" s="68"/>
-      <c r="T30" s="68"/>
-      <c r="U30" s="68"/>
-      <c r="V30" s="68"/>
+      <c r="S30" s="58"/>
+      <c r="T30" s="58"/>
+      <c r="U30" s="58"/>
+      <c r="V30" s="58"/>
       <c r="W30" s="3">
         <v>20</v>
       </c>
@@ -5339,91 +5339,91 @@
       <c r="X37" s="11"/>
     </row>
     <row r="38" spans="1:28" ht="14.25" customHeight="1">
-      <c r="B38" s="63" t="s">
+      <c r="B38" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="64"/>
-      <c r="D38" s="64"/>
-      <c r="E38" s="64"/>
-      <c r="F38" s="64"/>
-      <c r="G38" s="64"/>
-      <c r="H38" s="65"/>
+      <c r="C38" s="60"/>
+      <c r="D38" s="60"/>
+      <c r="E38" s="60"/>
+      <c r="F38" s="60"/>
+      <c r="G38" s="60"/>
+      <c r="H38" s="61"/>
       <c r="I38" s="16"/>
-      <c r="J38" s="63" t="s">
+      <c r="J38" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="K38" s="64"/>
-      <c r="L38" s="64"/>
-      <c r="M38" s="64"/>
-      <c r="N38" s="64"/>
-      <c r="O38" s="64"/>
-      <c r="P38" s="65"/>
+      <c r="K38" s="60"/>
+      <c r="L38" s="60"/>
+      <c r="M38" s="60"/>
+      <c r="N38" s="60"/>
+      <c r="O38" s="60"/>
+      <c r="P38" s="61"/>
       <c r="Q38" s="16"/>
-      <c r="R38" s="63" t="s">
+      <c r="R38" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="S38" s="64"/>
-      <c r="T38" s="64"/>
-      <c r="U38" s="64"/>
-      <c r="V38" s="64"/>
-      <c r="W38" s="64"/>
-      <c r="X38" s="65"/>
+      <c r="S38" s="60"/>
+      <c r="T38" s="60"/>
+      <c r="U38" s="60"/>
+      <c r="V38" s="60"/>
+      <c r="W38" s="60"/>
+      <c r="X38" s="61"/>
     </row>
     <row r="39" spans="1:28" ht="14.25" customHeight="1">
       <c r="B39" s="17">
         <v>13</v>
       </c>
-      <c r="C39" s="55" t="s">
+      <c r="C39" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="56"/>
-      <c r="G39" s="56"/>
-      <c r="H39" s="57"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="50"/>
+      <c r="H39" s="51"/>
       <c r="I39" s="18"/>
       <c r="J39" s="17">
         <v>3</v>
       </c>
-      <c r="K39" s="55" t="s">
+      <c r="K39" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="L39" s="56"/>
-      <c r="M39" s="56"/>
-      <c r="N39" s="56"/>
-      <c r="O39" s="56"/>
-      <c r="P39" s="57"/>
+      <c r="L39" s="50"/>
+      <c r="M39" s="50"/>
+      <c r="N39" s="50"/>
+      <c r="O39" s="50"/>
+      <c r="P39" s="51"/>
       <c r="Q39" s="18"/>
-      <c r="R39" s="66" t="s">
+      <c r="R39" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="S39" s="56"/>
-      <c r="T39" s="56"/>
-      <c r="U39" s="56"/>
-      <c r="V39" s="56"/>
-      <c r="W39" s="56"/>
-      <c r="X39" s="57"/>
+      <c r="S39" s="50"/>
+      <c r="T39" s="50"/>
+      <c r="U39" s="50"/>
+      <c r="V39" s="50"/>
+      <c r="W39" s="50"/>
+      <c r="X39" s="51"/>
     </row>
     <row r="40" spans="1:28" ht="14.25" customHeight="1">
       <c r="B40" s="21"/>
-      <c r="C40" s="69"/>
-      <c r="D40" s="56"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="56"/>
-      <c r="G40" s="56"/>
-      <c r="H40" s="57"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="50"/>
+      <c r="H40" s="51"/>
       <c r="I40" s="18"/>
       <c r="J40" s="22">
         <v>24</v>
       </c>
-      <c r="K40" s="58" t="s">
+      <c r="K40" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="L40" s="59"/>
-      <c r="M40" s="59"/>
-      <c r="N40" s="59"/>
-      <c r="O40" s="59"/>
-      <c r="P40" s="60"/>
+      <c r="L40" s="53"/>
+      <c r="M40" s="53"/>
+      <c r="N40" s="53"/>
+      <c r="O40" s="53"/>
+      <c r="P40" s="54"/>
       <c r="Q40" s="18"/>
       <c r="R40" s="35"/>
       <c r="S40" s="36"/>
@@ -5434,29 +5434,29 @@
       <c r="X40" s="37"/>
     </row>
     <row r="41" spans="1:28" ht="13.5" customHeight="1">
-      <c r="B41" s="62"/>
-      <c r="C41" s="59"/>
-      <c r="D41" s="59"/>
-      <c r="E41" s="59"/>
-      <c r="F41" s="59"/>
-      <c r="G41" s="59"/>
-      <c r="H41" s="60"/>
+      <c r="B41" s="55"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="53"/>
+      <c r="F41" s="53"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="54"/>
       <c r="I41" s="26"/>
-      <c r="J41" s="62"/>
-      <c r="K41" s="59"/>
-      <c r="L41" s="59"/>
-      <c r="M41" s="59"/>
-      <c r="N41" s="59"/>
-      <c r="O41" s="59"/>
-      <c r="P41" s="60"/>
+      <c r="J41" s="55"/>
+      <c r="K41" s="53"/>
+      <c r="L41" s="53"/>
+      <c r="M41" s="53"/>
+      <c r="N41" s="53"/>
+      <c r="O41" s="53"/>
+      <c r="P41" s="54"/>
       <c r="Q41" s="18"/>
       <c r="R41" s="30"/>
-      <c r="S41" s="70"/>
-      <c r="T41" s="59"/>
-      <c r="U41" s="59"/>
-      <c r="V41" s="59"/>
-      <c r="W41" s="59"/>
-      <c r="X41" s="60"/>
+      <c r="S41" s="56"/>
+      <c r="T41" s="53"/>
+      <c r="U41" s="53"/>
+      <c r="V41" s="53"/>
+      <c r="W41" s="53"/>
+      <c r="X41" s="54"/>
     </row>
     <row r="42" spans="1:28" ht="6" customHeight="1">
       <c r="B42" s="26"/>
@@ -5485,13 +5485,13 @@
     </row>
     <row r="43" spans="1:28" ht="14.25" customHeight="1">
       <c r="A43" s="2"/>
-      <c r="B43" s="67">
+      <c r="B43" s="57">
         <v>46023</v>
       </c>
-      <c r="C43" s="68"/>
-      <c r="D43" s="68"/>
-      <c r="E43" s="68"/>
-      <c r="F43" s="68"/>
+      <c r="C43" s="58"/>
+      <c r="D43" s="58"/>
+      <c r="E43" s="58"/>
+      <c r="F43" s="58"/>
       <c r="G43" s="3">
         <v>19</v>
       </c>
@@ -5499,13 +5499,13 @@
         <v>12</v>
       </c>
       <c r="I43" s="2"/>
-      <c r="J43" s="67">
+      <c r="J43" s="57">
         <v>46054</v>
       </c>
-      <c r="K43" s="68"/>
-      <c r="L43" s="68"/>
-      <c r="M43" s="68"/>
-      <c r="N43" s="68"/>
+      <c r="K43" s="58"/>
+      <c r="L43" s="58"/>
+      <c r="M43" s="58"/>
+      <c r="N43" s="58"/>
       <c r="O43" s="3">
         <v>20</v>
       </c>
@@ -5513,13 +5513,13 @@
         <v>8</v>
       </c>
       <c r="Q43" s="2"/>
-      <c r="R43" s="67">
+      <c r="R43" s="57">
         <v>46082</v>
       </c>
-      <c r="S43" s="68"/>
-      <c r="T43" s="68"/>
-      <c r="U43" s="68"/>
-      <c r="V43" s="68"/>
+      <c r="S43" s="58"/>
+      <c r="T43" s="58"/>
+      <c r="U43" s="58"/>
+      <c r="V43" s="58"/>
       <c r="W43" s="3">
         <v>22</v>
       </c>
@@ -5904,130 +5904,130 @@
       <c r="X49" s="11"/>
     </row>
     <row r="50" spans="2:28" ht="13.5" customHeight="1">
-      <c r="B50" s="63" t="s">
+      <c r="B50" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="64"/>
-      <c r="D50" s="64"/>
-      <c r="E50" s="64"/>
-      <c r="F50" s="64"/>
-      <c r="G50" s="64"/>
-      <c r="H50" s="65"/>
+      <c r="C50" s="60"/>
+      <c r="D50" s="60"/>
+      <c r="E50" s="60"/>
+      <c r="F50" s="60"/>
+      <c r="G50" s="60"/>
+      <c r="H50" s="61"/>
       <c r="I50" s="16"/>
-      <c r="J50" s="63" t="s">
+      <c r="J50" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="K50" s="64"/>
-      <c r="L50" s="64"/>
-      <c r="M50" s="64"/>
-      <c r="N50" s="64"/>
-      <c r="O50" s="64"/>
-      <c r="P50" s="65"/>
+      <c r="K50" s="60"/>
+      <c r="L50" s="60"/>
+      <c r="M50" s="60"/>
+      <c r="N50" s="60"/>
+      <c r="O50" s="60"/>
+      <c r="P50" s="61"/>
       <c r="Q50" s="16"/>
-      <c r="R50" s="63" t="s">
+      <c r="R50" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="S50" s="64"/>
-      <c r="T50" s="64"/>
-      <c r="U50" s="64"/>
-      <c r="V50" s="64"/>
-      <c r="W50" s="64"/>
-      <c r="X50" s="65"/>
+      <c r="S50" s="60"/>
+      <c r="T50" s="60"/>
+      <c r="U50" s="60"/>
+      <c r="V50" s="60"/>
+      <c r="W50" s="60"/>
+      <c r="X50" s="61"/>
     </row>
     <row r="51" spans="2:28" ht="13.5" customHeight="1">
       <c r="B51" s="17">
         <v>1</v>
       </c>
-      <c r="C51" s="55" t="s">
+      <c r="C51" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="D51" s="56"/>
-      <c r="E51" s="56"/>
-      <c r="F51" s="56"/>
-      <c r="G51" s="56"/>
-      <c r="H51" s="57"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="50"/>
+      <c r="F51" s="50"/>
+      <c r="G51" s="50"/>
+      <c r="H51" s="51"/>
       <c r="I51" s="18"/>
       <c r="J51" s="17">
         <v>11</v>
       </c>
-      <c r="K51" s="55" t="s">
+      <c r="K51" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="L51" s="56"/>
-      <c r="M51" s="56"/>
-      <c r="N51" s="56"/>
-      <c r="O51" s="56"/>
-      <c r="P51" s="57"/>
+      <c r="L51" s="50"/>
+      <c r="M51" s="50"/>
+      <c r="N51" s="50"/>
+      <c r="O51" s="50"/>
+      <c r="P51" s="51"/>
       <c r="Q51" s="18"/>
       <c r="R51" s="17">
         <v>20</v>
       </c>
-      <c r="S51" s="55" t="s">
+      <c r="S51" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="T51" s="56"/>
-      <c r="U51" s="56"/>
-      <c r="V51" s="56"/>
-      <c r="W51" s="56"/>
-      <c r="X51" s="57"/>
+      <c r="T51" s="50"/>
+      <c r="U51" s="50"/>
+      <c r="V51" s="50"/>
+      <c r="W51" s="50"/>
+      <c r="X51" s="51"/>
     </row>
     <row r="52" spans="2:28" ht="14.25" customHeight="1">
       <c r="B52" s="22">
         <v>12</v>
       </c>
-      <c r="C52" s="58" t="s">
+      <c r="C52" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="D52" s="59"/>
-      <c r="E52" s="59"/>
-      <c r="F52" s="59"/>
-      <c r="G52" s="59"/>
-      <c r="H52" s="60"/>
+      <c r="D52" s="53"/>
+      <c r="E52" s="53"/>
+      <c r="F52" s="53"/>
+      <c r="G52" s="53"/>
+      <c r="H52" s="54"/>
       <c r="I52" s="18"/>
       <c r="J52" s="17">
         <v>23</v>
       </c>
-      <c r="K52" s="55" t="s">
+      <c r="K52" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="L52" s="56"/>
-      <c r="M52" s="56"/>
-      <c r="N52" s="56"/>
-      <c r="O52" s="56"/>
-      <c r="P52" s="57"/>
+      <c r="L52" s="50"/>
+      <c r="M52" s="50"/>
+      <c r="N52" s="50"/>
+      <c r="O52" s="50"/>
+      <c r="P52" s="51"/>
       <c r="Q52" s="18"/>
-      <c r="R52" s="61"/>
-      <c r="S52" s="56"/>
-      <c r="T52" s="56"/>
-      <c r="U52" s="56"/>
-      <c r="V52" s="56"/>
-      <c r="W52" s="56"/>
-      <c r="X52" s="57"/>
+      <c r="R52" s="63"/>
+      <c r="S52" s="50"/>
+      <c r="T52" s="50"/>
+      <c r="U52" s="50"/>
+      <c r="V52" s="50"/>
+      <c r="W52" s="50"/>
+      <c r="X52" s="51"/>
     </row>
     <row r="53" spans="2:28" ht="13.5" customHeight="1">
-      <c r="B53" s="62"/>
-      <c r="C53" s="59"/>
-      <c r="D53" s="59"/>
-      <c r="E53" s="59"/>
-      <c r="F53" s="59"/>
-      <c r="G53" s="59"/>
-      <c r="H53" s="60"/>
+      <c r="B53" s="55"/>
+      <c r="C53" s="53"/>
+      <c r="D53" s="53"/>
+      <c r="E53" s="53"/>
+      <c r="F53" s="53"/>
+      <c r="G53" s="53"/>
+      <c r="H53" s="54"/>
       <c r="I53" s="18"/>
-      <c r="J53" s="62"/>
-      <c r="K53" s="59"/>
-      <c r="L53" s="59"/>
-      <c r="M53" s="59"/>
-      <c r="N53" s="59"/>
-      <c r="O53" s="59"/>
-      <c r="P53" s="60"/>
+      <c r="J53" s="55"/>
+      <c r="K53" s="53"/>
+      <c r="L53" s="53"/>
+      <c r="M53" s="53"/>
+      <c r="N53" s="53"/>
+      <c r="O53" s="53"/>
+      <c r="P53" s="54"/>
       <c r="Q53" s="26"/>
-      <c r="R53" s="62"/>
-      <c r="S53" s="59"/>
-      <c r="T53" s="59"/>
-      <c r="U53" s="59"/>
-      <c r="V53" s="59"/>
-      <c r="W53" s="59"/>
-      <c r="X53" s="60"/>
+      <c r="R53" s="55"/>
+      <c r="S53" s="53"/>
+      <c r="T53" s="53"/>
+      <c r="U53" s="53"/>
+      <c r="V53" s="53"/>
+      <c r="W53" s="53"/>
+      <c r="X53" s="54"/>
     </row>
     <row r="54" spans="2:28" ht="13.5" customHeight="1">
       <c r="Z54" s="38" t="s">
@@ -6125,11 +6125,11 @@
       <c r="S57" s="43"/>
       <c r="T57" s="43"/>
       <c r="U57" s="43"/>
-      <c r="V57" s="49" t="s">
+      <c r="V57" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="W57" s="50"/>
-      <c r="X57" s="51"/>
+      <c r="W57" s="69"/>
+      <c r="X57" s="70"/>
       <c r="Z57" s="38" t="s">
         <v>39</v>
       </c>
@@ -6148,11 +6148,11 @@
       <c r="S58" s="43"/>
       <c r="T58" s="43"/>
       <c r="U58" s="43"/>
-      <c r="V58" s="52">
+      <c r="V58" s="71">
         <v>0</v>
       </c>
-      <c r="W58" s="50"/>
-      <c r="X58" s="51"/>
+      <c r="W58" s="69"/>
+      <c r="X58" s="70"/>
       <c r="Z58" s="38" t="s">
         <v>40</v>
       </c>
@@ -6163,16 +6163,16 @@
     <row r="59" spans="2:28" ht="13.5" customHeight="1">
       <c r="B59" s="46"/>
       <c r="C59" s="41"/>
-      <c r="O59" s="53"/>
-      <c r="P59" s="54"/>
-      <c r="Q59" s="54"/>
-      <c r="R59" s="54"/>
-      <c r="S59" s="54"/>
-      <c r="T59" s="54"/>
-      <c r="U59" s="54"/>
-      <c r="V59" s="54"/>
-      <c r="W59" s="54"/>
-      <c r="X59" s="54"/>
+      <c r="O59" s="72"/>
+      <c r="P59" s="66"/>
+      <c r="Q59" s="66"/>
+      <c r="R59" s="66"/>
+      <c r="S59" s="66"/>
+      <c r="T59" s="66"/>
+      <c r="U59" s="66"/>
+      <c r="V59" s="66"/>
+      <c r="W59" s="66"/>
+      <c r="X59" s="66"/>
     </row>
     <row r="60" spans="2:28" ht="13.5" customHeight="1">
       <c r="B60" s="46"/>
@@ -7297,40 +7297,24 @@
     <row r="1000" ht="13.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="K40:P40"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="J41:P41"/>
-    <mergeCell ref="S41:X41"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="J43:N43"/>
-    <mergeCell ref="R43:V43"/>
-    <mergeCell ref="B50:H50"/>
-    <mergeCell ref="J50:P50"/>
-    <mergeCell ref="R50:X50"/>
-    <mergeCell ref="J17:N17"/>
-    <mergeCell ref="R17:V17"/>
-    <mergeCell ref="R12:X12"/>
-    <mergeCell ref="R13:X13"/>
-    <mergeCell ref="J25:P25"/>
-    <mergeCell ref="R25:X25"/>
-    <mergeCell ref="K12:P12"/>
-    <mergeCell ref="K13:P13"/>
-    <mergeCell ref="K14:P14"/>
-    <mergeCell ref="K15:P15"/>
-    <mergeCell ref="R15:X15"/>
-    <mergeCell ref="C2:X2"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="J4:N4"/>
-    <mergeCell ref="R4:V4"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="R11:X11"/>
-    <mergeCell ref="J11:P11"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="V57:X57"/>
+    <mergeCell ref="V58:X58"/>
+    <mergeCell ref="O59:X59"/>
+    <mergeCell ref="C51:H51"/>
+    <mergeCell ref="C52:H52"/>
+    <mergeCell ref="K52:P52"/>
+    <mergeCell ref="R52:X52"/>
+    <mergeCell ref="B53:H53"/>
+    <mergeCell ref="J53:P53"/>
+    <mergeCell ref="R53:X53"/>
+    <mergeCell ref="K51:P51"/>
+    <mergeCell ref="S51:X51"/>
+    <mergeCell ref="B38:H38"/>
+    <mergeCell ref="J38:P38"/>
+    <mergeCell ref="R38:X38"/>
+    <mergeCell ref="K39:P39"/>
+    <mergeCell ref="R39:X39"/>
+    <mergeCell ref="C39:H39"/>
     <mergeCell ref="J30:N30"/>
     <mergeCell ref="R30:V30"/>
     <mergeCell ref="B25:H25"/>
@@ -7344,24 +7328,40 @@
     <mergeCell ref="B30:F30"/>
     <mergeCell ref="J27:P27"/>
     <mergeCell ref="K28:P28"/>
-    <mergeCell ref="B38:H38"/>
-    <mergeCell ref="J38:P38"/>
-    <mergeCell ref="R38:X38"/>
-    <mergeCell ref="K39:P39"/>
-    <mergeCell ref="R39:X39"/>
-    <mergeCell ref="C39:H39"/>
-    <mergeCell ref="V57:X57"/>
-    <mergeCell ref="V58:X58"/>
-    <mergeCell ref="O59:X59"/>
-    <mergeCell ref="C51:H51"/>
-    <mergeCell ref="C52:H52"/>
-    <mergeCell ref="K52:P52"/>
-    <mergeCell ref="R52:X52"/>
-    <mergeCell ref="B53:H53"/>
-    <mergeCell ref="J53:P53"/>
-    <mergeCell ref="R53:X53"/>
-    <mergeCell ref="K51:P51"/>
-    <mergeCell ref="S51:X51"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="C2:X2"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="J4:N4"/>
+    <mergeCell ref="R4:V4"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="R11:X11"/>
+    <mergeCell ref="J11:P11"/>
+    <mergeCell ref="J17:N17"/>
+    <mergeCell ref="R17:V17"/>
+    <mergeCell ref="R12:X12"/>
+    <mergeCell ref="R13:X13"/>
+    <mergeCell ref="J25:P25"/>
+    <mergeCell ref="R25:X25"/>
+    <mergeCell ref="K12:P12"/>
+    <mergeCell ref="K13:P13"/>
+    <mergeCell ref="K14:P14"/>
+    <mergeCell ref="K15:P15"/>
+    <mergeCell ref="R15:X15"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="J43:N43"/>
+    <mergeCell ref="R43:V43"/>
+    <mergeCell ref="B50:H50"/>
+    <mergeCell ref="J50:P50"/>
+    <mergeCell ref="R50:X50"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="K40:P40"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="J41:P41"/>
+    <mergeCell ref="S41:X41"/>
   </mergeCells>
   <phoneticPr fontId="10"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>